<commit_message>
Fixed screenshot funktion til kun at tage billede af nuværende vindue og gemme som png.
</commit_message>
<xml_diff>
--- a/Uddeholm.Test/bin/debug/toerstraaling.xlsx
+++ b/Uddeholm.Test/bin/debug/toerstraaling.xlsx
@@ -1,18 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17809"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="4" documentId="53BB53B4ECCF1451F47A04323D4BA41F8B889B1E" xr6:coauthVersionLast="12" xr6:coauthVersionMax="12" xr10:uidLastSave="{A9911C0E-2C87-421F-93B0-83C4348877D7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="171026"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Til og med cm³</t>
   </si>
@@ -62,9 +58,6 @@
       </rPr>
       <t xml:space="preserve"> stk. DKK/stk</t>
     </r>
-  </si>
-  <si>
-    <t>This cell has an external reference that can't be shown or edited. Editing this cell will remove the external reference.</t>
   </si>
   <si>
     <t>Kurs omregn</t>
@@ -132,8 +125,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -543,171 +536,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="PL_DKK_20161101"/>
-      <sheetName val="INFO"/>
-      <sheetName val="PL_EURO"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="8">
-          <cell r="G8">
-            <v>7.5</v>
-          </cell>
-          <cell r="H8">
-            <v>1.25</v>
-          </cell>
-          <cell r="I8">
-            <v>1.1499999999999999</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="10">
-          <cell r="B10">
-            <v>1.53</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>2.04</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>2.5499999999999998</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>3.06</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>3.57</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>4.08</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16">
-            <v>5.0999999999999996</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17">
-            <v>6.12</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18">
-            <v>6.63</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19">
-            <v>7.65</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20">
-            <v>8.67</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21">
-            <v>10.199999999999999</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22">
-            <v>12.25</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23">
-            <v>14.7</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24">
-            <v>17.64</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25">
-            <v>21.17</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26">
-            <v>25.4</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="B27">
-            <v>30.48</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28">
-            <v>36.58</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29">
-            <v>43.9</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30">
-            <v>52.68</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="B31">
-            <v>63.22</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="B32">
-            <v>75.86</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="B33">
-            <v>91.03</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="B34">
-            <v>109.24</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="B35">
-            <v>131.09</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="B36">
-            <v>157.30000000000001</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1006,19 +834,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="4"/>
+    <col min="1" max="16384" width="11.44140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.9" thickBot="1">
+    <row r="1" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1032,138 +860,118 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.45">
+    <row r="2" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>50.09</v>
       </c>
       <c r="B2" s="6">
-        <f t="shared" ref="B2:B28" si="0">+$H$13+D2</f>
         <v>66.495312499999997</v>
       </c>
       <c r="C2" s="7">
-        <f t="shared" ref="C2:C28" si="1">+$H$12+D2</f>
         <v>46.495312499999997</v>
       </c>
       <c r="D2" s="8">
-        <f>(+[1]PL_EURO!B10*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
-        <v>26.495312499999997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="14.45">
+        <v>26.495312500000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>100.09</v>
       </c>
       <c r="B3" s="10">
-        <f t="shared" si="0"/>
         <v>71.993750000000006</v>
       </c>
       <c r="C3" s="11">
-        <f t="shared" si="1"/>
         <v>51.993749999999999</v>
       </c>
       <c r="D3" s="12">
-        <f>(+[1]PL_EURO!B11*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
         <v>31.993749999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.45">
+    <row r="4" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>150.09</v>
       </c>
-      <c r="B4" s="14" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C4" s="7" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>4</v>
+      <c r="B4" s="14">
+        <v>77.4921875</v>
+      </c>
+      <c r="C4" s="7">
+        <v>57.4921875</v>
+      </c>
+      <c r="D4" s="8">
+        <v>37.4921875</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
     </row>
-    <row r="5" spans="1:9" ht="17.45">
+    <row r="5" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>200.09</v>
       </c>
       <c r="B5" s="10">
-        <f t="shared" si="0"/>
         <v>82.990624999999994</v>
       </c>
       <c r="C5" s="11">
-        <f t="shared" si="1"/>
-        <v>62.990624999999994</v>
+        <v>62.990625000000001</v>
       </c>
       <c r="D5" s="12">
-        <f>(+[1]PL_EURO!B13*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
-        <v>42.990624999999994</v>
+        <v>42.990625000000001</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="15"/>
     </row>
-    <row r="6" spans="1:9" ht="14.45">
+    <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>300.08999999999997</v>
       </c>
       <c r="B6" s="14">
-        <f t="shared" si="0"/>
-        <v>88.489062499999989</v>
+        <v>88.489062500000003</v>
       </c>
       <c r="C6" s="7">
-        <f t="shared" si="1"/>
-        <v>68.489062499999989</v>
+        <v>68.489062500000003</v>
       </c>
       <c r="D6" s="8">
-        <f>(+[1]PL_EURO!B14*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
-        <v>48.489062499999996</v>
+        <v>48.489062500000003</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>500.09</v>
       </c>
       <c r="B7" s="10">
-        <f t="shared" si="0"/>
         <v>93.987499999999997</v>
       </c>
       <c r="C7" s="11">
-        <f t="shared" si="1"/>
         <v>73.987499999999997</v>
       </c>
       <c r="D7" s="12">
-        <f>(+[1]PL_EURO!B15*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
         <v>53.987499999999997</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="15"/>
       <c r="G7" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="I7" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1">
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>750.09</v>
       </c>
       <c r="B8" s="14">
-        <f t="shared" si="0"/>
         <v>104.984375</v>
       </c>
       <c r="C8" s="7">
-        <f t="shared" si="1"/>
         <v>84.984375</v>
       </c>
       <c r="D8" s="8">
-        <f>(+[1]PL_EURO!B16*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
         <v>64.984375</v>
       </c>
       <c r="E8" s="20"/>
@@ -1178,383 +986,323 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.45">
+    <row r="9" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>1000.09</v>
       </c>
       <c r="B9" s="10">
-        <f t="shared" si="0"/>
-        <v>115.98124999999999</v>
+        <v>115.98125</v>
       </c>
       <c r="C9" s="11">
-        <f t="shared" si="1"/>
-        <v>95.981249999999989</v>
+        <v>95.981250000000003</v>
       </c>
       <c r="D9" s="12">
-        <f>(+[1]PL_EURO!B17*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
-        <v>75.981249999999989</v>
+        <v>75.981250000000003</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
       <c r="G9" s="24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
     </row>
-    <row r="10" spans="1:9" ht="14.45">
+    <row r="10" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>1500.09</v>
       </c>
       <c r="B10" s="14">
-        <f t="shared" si="0"/>
         <v>121.4796875</v>
       </c>
       <c r="C10" s="7">
-        <f t="shared" si="1"/>
         <v>101.4796875</v>
       </c>
       <c r="D10" s="8">
-        <f>(+[1]PL_EURO!B18*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
         <v>81.479687499999997</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H10" s="24">
         <v>10</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="14.45">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>2000.09</v>
       </c>
       <c r="B11" s="10">
-        <f t="shared" si="0"/>
         <v>132.4765625</v>
       </c>
       <c r="C11" s="11">
-        <f t="shared" si="1"/>
         <v>112.4765625</v>
       </c>
       <c r="D11" s="12">
-        <f>(+[1]PL_EURO!B19*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
         <v>92.4765625</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
     </row>
-    <row r="12" spans="1:9" ht="14.45">
+    <row r="12" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>3000.09</v>
       </c>
       <c r="B12" s="14">
-        <f t="shared" si="0"/>
         <v>143.47343749999999</v>
       </c>
       <c r="C12" s="7">
-        <f t="shared" si="1"/>
-        <v>123.47343749999999</v>
+        <v>123.4734375</v>
       </c>
       <c r="D12" s="8">
-        <f>(+[1]PL_EURO!B20*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
-        <v>103.47343749999999</v>
+        <v>103.4734375</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H12" s="26">
         <v>20</v>
       </c>
       <c r="I12" s="26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="14.45">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>4000.09</v>
       </c>
       <c r="B13" s="10">
-        <f t="shared" si="0"/>
         <v>159.96875</v>
       </c>
       <c r="C13" s="11">
-        <f t="shared" si="1"/>
         <v>139.96875</v>
       </c>
       <c r="D13" s="12">
-        <f>(+[1]PL_EURO!B21*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
-        <v>119.96874999999999</v>
+        <v>119.96875</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H13" s="26">
         <v>40</v>
       </c>
       <c r="I13" s="26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="14.45">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>5000.09</v>
       </c>
       <c r="B14" s="14">
-        <f t="shared" si="0"/>
         <v>182.0703125</v>
       </c>
       <c r="C14" s="7">
-        <f t="shared" si="1"/>
         <v>162.0703125</v>
       </c>
       <c r="D14" s="8">
-        <f>(+[1]PL_EURO!B22*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
         <v>142.0703125</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.45">
+    <row r="15" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>6000.09</v>
       </c>
       <c r="B15" s="10">
-        <f t="shared" si="0"/>
         <v>208.484375</v>
       </c>
       <c r="C15" s="11">
-        <f t="shared" si="1"/>
         <v>188.484375</v>
       </c>
       <c r="D15" s="12">
-        <f>(+[1]PL_EURO!B23*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
         <v>168.484375</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.45">
+    <row r="16" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>7000.09</v>
       </c>
       <c r="B16" s="14">
-        <f t="shared" si="0"/>
-        <v>240.18124999999998</v>
+        <v>240.18125000000001</v>
       </c>
       <c r="C16" s="7">
-        <f t="shared" si="1"/>
-        <v>220.18124999999998</v>
+        <v>220.18125000000001</v>
       </c>
       <c r="D16" s="8">
-        <f>(+[1]PL_EURO!B24*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
-        <v>200.18124999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="14.45">
+        <v>200.18125000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>8000.09</v>
       </c>
       <c r="B17" s="10">
-        <f t="shared" si="0"/>
         <v>278.23906249999999</v>
       </c>
       <c r="C17" s="11">
-        <f t="shared" si="1"/>
         <v>258.23906249999999</v>
       </c>
       <c r="D17" s="12">
-        <f>(+[1]PL_EURO!B25*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
         <v>238.23906249999999</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="14.45">
+    <row r="18" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>9000.09</v>
       </c>
       <c r="B18" s="14">
-        <f t="shared" si="0"/>
         <v>323.84375</v>
       </c>
       <c r="C18" s="7">
-        <f t="shared" si="1"/>
         <v>303.84375</v>
       </c>
       <c r="D18" s="8">
-        <f>(+[1]PL_EURO!B26*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
         <v>283.84375</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="14.45">
+    <row r="19" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>10000.09</v>
       </c>
       <c r="B19" s="10">
-        <f t="shared" si="0"/>
-        <v>378.61249999999995</v>
+        <v>378.61250000000001</v>
       </c>
       <c r="C19" s="11">
-        <f t="shared" si="1"/>
-        <v>358.61249999999995</v>
+        <v>358.61250000000001</v>
       </c>
       <c r="D19" s="12">
-        <f>(+[1]PL_EURO!B27*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
-        <v>338.61249999999995</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="14.45">
+        <v>338.61250000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>11000.09</v>
       </c>
       <c r="B20" s="14">
-        <f t="shared" si="0"/>
-        <v>444.3781249999999</v>
+        <v>444.37812500000001</v>
       </c>
       <c r="C20" s="7">
-        <f t="shared" si="1"/>
-        <v>424.3781249999999</v>
+        <v>424.37812500000001</v>
       </c>
       <c r="D20" s="8">
-        <f>(+[1]PL_EURO!B28*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
-        <v>404.3781249999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="14.45">
+        <v>404.37812500000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>12000.09</v>
       </c>
       <c r="B21" s="10">
-        <f t="shared" si="0"/>
         <v>523.296875</v>
       </c>
       <c r="C21" s="11">
-        <f t="shared" si="1"/>
-        <v>503.29687499999994</v>
+        <v>503.296875</v>
       </c>
       <c r="D21" s="12">
-        <f>(+[1]PL_EURO!B29*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
-        <v>483.29687499999994</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="14.45">
+        <v>483.296875</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>13000.09</v>
       </c>
       <c r="B22" s="14">
-        <f t="shared" si="0"/>
         <v>617.95624999999995</v>
       </c>
       <c r="C22" s="7">
-        <f t="shared" si="1"/>
         <v>597.95624999999995</v>
       </c>
       <c r="D22" s="8">
-        <f>(+[1]PL_EURO!B30*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
         <v>577.95624999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="14.45">
+    <row r="23" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>15000.09</v>
       </c>
       <c r="B23" s="10">
-        <f t="shared" si="0"/>
-        <v>731.59062499999993</v>
+        <v>731.59062500000005</v>
       </c>
       <c r="C23" s="11">
-        <f t="shared" si="1"/>
-        <v>711.59062499999993</v>
+        <v>711.59062500000005</v>
       </c>
       <c r="D23" s="12">
-        <f>(+[1]PL_EURO!B31*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
-        <v>691.59062499999993</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="14.45">
+        <v>691.59062500000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>20000.09</v>
       </c>
       <c r="B24" s="14">
-        <f t="shared" si="0"/>
-        <v>867.86562499999991</v>
+        <v>867.86562500000002</v>
       </c>
       <c r="C24" s="7">
-        <f t="shared" si="1"/>
-        <v>847.86562499999991</v>
+        <v>847.86562500000002</v>
       </c>
       <c r="D24" s="8">
-        <f>(+[1]PL_EURO!B32*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
-        <v>827.86562499999991</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="14.45">
+        <v>827.86562500000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>25000.09</v>
       </c>
       <c r="B25" s="10">
-        <f t="shared" si="0"/>
         <v>1031.4171875</v>
       </c>
       <c r="C25" s="11">
-        <f t="shared" si="1"/>
         <v>1011.4171875</v>
       </c>
       <c r="D25" s="12">
-        <f>(+[1]PL_EURO!B33*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
         <v>991.41718749999995</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="14.45">
+    <row r="26" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>30000.09</v>
       </c>
       <c r="B26" s="14">
-        <f t="shared" si="0"/>
-        <v>1227.7437499999999</v>
+        <v>1227.7437500000001</v>
       </c>
       <c r="C26" s="7">
-        <f t="shared" si="1"/>
-        <v>1207.7437499999999</v>
+        <v>1207.7437500000001</v>
       </c>
       <c r="D26" s="8">
-        <f>(+[1]PL_EURO!B34*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
-        <v>1187.7437499999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="14.45">
+        <v>1187.7437500000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>35000.089999999997</v>
       </c>
       <c r="B27" s="10">
-        <f t="shared" si="0"/>
-        <v>1463.3140624999999</v>
+        <v>1463.3140625000001</v>
       </c>
       <c r="C27" s="11">
-        <f t="shared" si="1"/>
-        <v>1443.3140624999999</v>
+        <v>1443.3140625000001</v>
       </c>
       <c r="D27" s="12">
-        <f>(+[1]PL_EURO!B35*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
-        <v>1423.3140624999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" thickBot="1">
+        <v>1423.3140625000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="27">
         <v>40000.089999999997</v>
       </c>
       <c r="B28" s="28">
-        <f t="shared" si="0"/>
-        <v>1745.8906249999998</v>
+        <v>1745.890625</v>
       </c>
       <c r="C28" s="29">
-        <f t="shared" si="1"/>
-        <v>1725.8906249999998</v>
+        <v>1725.890625</v>
       </c>
       <c r="D28" s="30">
-        <f>(+[1]PL_EURO!B36*[1]PL_DKK_20161101!$G$8*[1]PL_DKK_20161101!$H$8*[1]PL_DKK_20161101!$I$8)+$H$10</f>
-        <v>1705.8906249999998</v>
+        <v>1705.890625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>